<commit_message>
Add Regional and Topic Subteams
</commit_message>
<xml_diff>
--- a/data/objectives.xlsx
+++ b/data/objectives.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{C40C9DDC-1DCA-4AF0-965C-DCDDAB365C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32627A2D-7D98-4494-AE89-E101078B77AF}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{C40C9DDC-1DCA-4AF0-965C-DCDDAB365C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6073F385-3A04-46B0-9F16-CDBDE3233E5D}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3040" windowWidth="18000" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>objective</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>NorthAmerica</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>* Contribute China-specific regulatory and clinical practice perspectives
+* Develop and share practical case studies and implementation examples
+* Promote cross-functional understanding and adoption of the estimand framework
+* Collaborate on harmonized methodological and operational recommendations</t>
   </si>
 </sst>
 </file>
@@ -183,8 +192,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C729CC4F-0171-44B4-98D9-3794236DA206}" name="Tabelle1" displayName="Tabelle1" ref="A1:B11" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:B11" xr:uid="{C729CC4F-0171-44B4-98D9-3794236DA206}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C729CC4F-0171-44B4-98D9-3794236DA206}" name="Tabelle1" displayName="Tabelle1" ref="A1:B12" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:B12" xr:uid="{C729CC4F-0171-44B4-98D9-3794236DA206}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B7C46663-E00D-4705-B667-5C71EF2D208A}" name="subteams" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{A3B71FBA-B7BA-40FC-B396-D279C48A7CA4}" name="objective" dataDxfId="0"/>
@@ -456,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,6 +565,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="12" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>